<commit_message>
modified:   src/main/java/tools/datagen/GenerateTestCaseVariations.java modified:   src/main/java/tools/datagen/PopulateFeatureExamples.java 	modified:   test_files/SP_ID.xlsx
</commit_message>
<xml_diff>
--- a/test_files/SP_ID.xlsx
+++ b/test_files/SP_ID.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="20475" windowHeight="6990"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="18360" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -46,9 +46,6 @@
     <t>AST - Applied Satellite Technology (OPENPORT)</t>
   </si>
   <si>
-    <t>Speedcast France SAS</t>
-  </si>
-  <si>
     <t>Global Satellite FWI</t>
   </si>
   <si>
@@ -968,6 +965,9 @@
   </si>
   <si>
     <t>China Telecom (Roaming)</t>
+  </si>
+  <si>
+    <t>SpeedCast France SAS</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:B319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,15 +1363,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>315</v>
       </c>
       <c r="B9">
         <v>100983</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B10">
         <v>100984</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>100985</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>100986</v>
@@ -1395,7 +1395,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>100987</v>
@@ -1403,7 +1403,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>100989</v>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>100991</v>
@@ -1419,7 +1419,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>100992</v>
@@ -1427,7 +1427,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>100993</v>
@@ -1435,7 +1435,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>100997</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>100998</v>
@@ -1451,7 +1451,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>100999</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21">
         <v>101002</v>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22">
         <v>101003</v>
@@ -1475,7 +1475,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23">
         <v>101005</v>
@@ -1483,7 +1483,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24">
         <v>101006</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25">
         <v>101007</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>101010</v>
@@ -1507,7 +1507,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>101014</v>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>101015</v>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29">
         <v>101016</v>
@@ -1531,7 +1531,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>101018</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31">
         <v>101019</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>101020</v>
@@ -1555,7 +1555,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33">
         <v>101021</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34">
         <v>101025</v>
@@ -1571,7 +1571,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>101026</v>
@@ -1579,7 +1579,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
         <v>101027</v>
@@ -1587,7 +1587,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
         <v>101028</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
         <v>101029</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>101033</v>
@@ -1611,7 +1611,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
         <v>101034</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>101036</v>
@@ -1627,7 +1627,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42">
         <v>101041</v>
@@ -1635,7 +1635,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43">
         <v>101044</v>
@@ -1643,7 +1643,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44">
         <v>101045</v>
@@ -1651,7 +1651,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45">
         <v>101050</v>
@@ -1659,7 +1659,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46">
         <v>101055</v>
@@ -1667,7 +1667,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47">
         <v>101056</v>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48">
         <v>101064</v>
@@ -1683,7 +1683,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49">
         <v>101065</v>
@@ -1691,7 +1691,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50">
         <v>101068</v>
@@ -1699,7 +1699,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51">
         <v>101072</v>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52">
         <v>101073</v>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
         <v>101074</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
         <v>101076</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
         <v>101078</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
         <v>101080</v>
@@ -1747,7 +1747,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
         <v>101081</v>
@@ -1755,7 +1755,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
         <v>101082</v>
@@ -1763,7 +1763,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
         <v>101083</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <v>101084</v>
@@ -1779,7 +1779,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
         <v>101085</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
         <v>101086</v>
@@ -1795,7 +1795,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
         <v>101087</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
         <v>101088</v>
@@ -1811,7 +1811,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65">
         <v>101090</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66">
         <v>101091</v>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67">
         <v>101092</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68">
         <v>101094</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>101095</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70">
         <v>101098</v>
@@ -1859,7 +1859,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71">
         <v>101099</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>101102</v>
@@ -1875,7 +1875,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73">
         <v>101103</v>
@@ -1883,7 +1883,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74">
         <v>101104</v>
@@ -1891,7 +1891,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75">
         <v>101105</v>
@@ -1899,7 +1899,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76">
         <v>101106</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77">
         <v>101107</v>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78">
         <v>101108</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79">
         <v>101110</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80">
         <v>101111</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81">
         <v>101112</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82">
         <v>101115</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83">
         <v>101116</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84">
         <v>101117</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85">
         <v>101118</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86">
         <v>101120</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87">
         <v>101123</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88">
         <v>101124</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89">
         <v>101125</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90">
         <v>101126</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91">
         <v>101127</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92">
         <v>101128</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93">
         <v>101129</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94">
         <v>101130</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>101131</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96">
         <v>101137</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97">
         <v>101138</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98">
         <v>101139</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99">
         <v>101140</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100">
         <v>101141</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>101143</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102">
         <v>101144</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103">
         <v>101145</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104">
         <v>101146</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105">
         <v>101147</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106">
         <v>101148</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107">
         <v>101150</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108">
         <v>101151</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>101152</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110">
         <v>101153</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111">
         <v>101155</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112">
         <v>101156</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113">
         <v>101157</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114">
         <v>101158</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115">
         <v>101159</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116">
         <v>101160</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117">
         <v>101162</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118">
         <v>101164</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119">
         <v>101166</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120">
         <v>101167</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121">
         <v>101168</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122">
         <v>101169</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123">
         <v>101170</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124">
         <v>101171</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125">
         <v>101172</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126">
         <v>101174</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127">
         <v>101175</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128">
         <v>101177</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129">
         <v>101178</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130">
         <v>101179</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>101180</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132">
         <v>101184</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>101185</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134">
         <v>101186</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>101187</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136">
         <v>101188</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>101191</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138">
         <v>101192</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139">
         <v>101196</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140">
         <v>101197</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141">
         <v>101199</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142">
         <v>101200</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143">
         <v>101201</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144">
         <v>101202</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145">
         <v>101203</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B146">
         <v>101204</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147">
         <v>101205</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148">
         <v>101207</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B149">
         <v>101208</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B150">
         <v>101210</v>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151">
         <v>101215</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152">
         <v>101220</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153">
         <v>101222</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154">
         <v>101225</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155">
         <v>101227</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>101228</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157">
         <v>101229</v>
@@ -2555,7 +2555,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158">
         <v>101230</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159">
         <v>101231</v>
@@ -2571,7 +2571,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160">
         <v>101232</v>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161">
         <v>101233</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162">
         <v>101234</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163">
         <v>101235</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164">
         <v>101236</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165">
         <v>101237</v>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166">
         <v>101238</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167">
         <v>101240</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168">
         <v>101242</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169">
         <v>101243</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170">
         <v>101245</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171">
         <v>101246</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172">
         <v>101247</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173">
         <v>101248</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174">
         <v>200001</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175">
         <v>200002</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176">
         <v>200008</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B177">
         <v>200014</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178">
         <v>200016</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B179">
         <v>200018</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180">
         <v>200019</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181">
         <v>200252</v>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182">
         <v>200253</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183">
         <v>200256</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184">
         <v>200257</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185">
         <v>200259</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B186">
         <v>200260</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B187">
         <v>200261</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188">
         <v>200262</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189">
         <v>200264</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190">
         <v>200265</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191">
         <v>200268</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192">
         <v>200269</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193">
         <v>200270</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194">
         <v>200271</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B195">
         <v>200274</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B196">
         <v>200275</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B197">
         <v>200276</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B198">
         <v>200277</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199">
         <v>200278</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200">
         <v>200280</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201">
         <v>200281</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202">
         <v>200282</v>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203">
         <v>200283</v>
@@ -2923,7 +2923,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204">
         <v>200287</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205">
         <v>200291</v>
@@ -2939,7 +2939,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206">
         <v>200292</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207">
         <v>200293</v>
@@ -2960,7 +2960,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B209">
         <v>200295</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B210">
         <v>200296</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B211">
         <v>200301</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B212">
         <v>200306</v>
@@ -2992,7 +2992,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B213">
         <v>200308</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B214">
         <v>200310</v>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B215">
         <v>200312</v>
@@ -3016,7 +3016,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B216">
         <v>200313</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B217">
         <v>200342</v>
@@ -3032,7 +3032,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B218">
         <v>200344</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B219">
         <v>200350</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B220">
         <v>200355</v>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B221">
         <v>200356</v>
@@ -3064,7 +3064,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B222">
         <v>200360</v>
@@ -3072,7 +3072,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B223">
         <v>200365</v>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B224">
         <v>200367</v>
@@ -3088,7 +3088,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B225">
         <v>200368</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B226">
         <v>200377</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B227">
         <v>200380</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B228">
         <v>200381</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B229">
         <v>200382</v>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B230">
         <v>200391</v>
@@ -3136,7 +3136,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B231">
         <v>200414</v>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B232">
         <v>200415</v>
@@ -3152,7 +3152,7 @@
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B233">
         <v>200416</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B234">
         <v>200419</v>
@@ -3168,7 +3168,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B235">
         <v>200420</v>
@@ -3176,7 +3176,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B236">
         <v>200421</v>
@@ -3184,7 +3184,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B237">
         <v>200426</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B238">
         <v>200427</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B239">
         <v>200428</v>
@@ -3208,7 +3208,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B240">
         <v>200429</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B241">
         <v>200430</v>
@@ -3224,7 +3224,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B242">
         <v>200431</v>
@@ -3232,7 +3232,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B243">
         <v>200433</v>
@@ -3240,7 +3240,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B244">
         <v>200434</v>
@@ -3248,7 +3248,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B245">
         <v>200436</v>
@@ -3256,7 +3256,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B246">
         <v>200438</v>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B247">
         <v>200439</v>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B248">
         <v>200440</v>
@@ -3280,7 +3280,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B249">
         <v>200441</v>
@@ -3288,7 +3288,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B250">
         <v>200446</v>
@@ -3296,7 +3296,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B251">
         <v>200449</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B252">
         <v>200450</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B253">
         <v>200451</v>
@@ -3320,7 +3320,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B254">
         <v>200456</v>
@@ -3328,7 +3328,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B255">
         <v>200459</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B256">
         <v>200463</v>
@@ -3344,7 +3344,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B257">
         <v>200464</v>
@@ -3352,7 +3352,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B258">
         <v>200465</v>
@@ -3360,7 +3360,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B259">
         <v>200466</v>
@@ -3368,7 +3368,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B260">
         <v>200467</v>
@@ -3376,7 +3376,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B261">
         <v>200470</v>
@@ -3384,7 +3384,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B262">
         <v>200471</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B263">
         <v>200475</v>
@@ -3400,7 +3400,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B264">
         <v>200476</v>
@@ -3408,7 +3408,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B265">
         <v>200477</v>
@@ -3416,7 +3416,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B266">
         <v>200478</v>
@@ -3424,7 +3424,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B267">
         <v>200479</v>
@@ -3432,7 +3432,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B268">
         <v>200480</v>
@@ -3440,7 +3440,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B269">
         <v>200483</v>
@@ -3448,7 +3448,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B270">
         <v>200484</v>
@@ -3456,7 +3456,7 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B271">
         <v>200485</v>
@@ -3464,7 +3464,7 @@
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B272">
         <v>200486</v>
@@ -3472,7 +3472,7 @@
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B273">
         <v>200487</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B274">
         <v>200488</v>
@@ -3488,7 +3488,7 @@
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B275">
         <v>200489</v>
@@ -3501,7 +3501,7 @@
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B277">
         <v>300028</v>
@@ -3509,7 +3509,7 @@
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B278">
         <v>300061</v>
@@ -3517,7 +3517,7 @@
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B279">
         <v>300066</v>
@@ -3525,7 +3525,7 @@
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B280">
         <v>300067</v>
@@ -3533,7 +3533,7 @@
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B281">
         <v>300068</v>
@@ -3541,7 +3541,7 @@
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B282">
         <v>300087</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B283">
         <v>300094</v>
@@ -3557,7 +3557,7 @@
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B284">
         <v>300354</v>
@@ -3565,7 +3565,7 @@
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B285">
         <v>300364</v>
@@ -3573,7 +3573,7 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B286">
         <v>300454</v>
@@ -3581,7 +3581,7 @@
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B287">
         <v>300455</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B288">
         <v>300456</v>
@@ -3597,7 +3597,7 @@
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B289">
         <v>300457</v>
@@ -3605,7 +3605,7 @@
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B290">
         <v>300458</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B291">
         <v>400001</v>
@@ -3621,7 +3621,7 @@
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B292">
         <v>400003</v>
@@ -3629,7 +3629,7 @@
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B293">
         <v>400004</v>
@@ -3637,7 +3637,7 @@
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B294">
         <v>400005</v>
@@ -3645,7 +3645,7 @@
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B295">
         <v>400007</v>
@@ -3653,7 +3653,7 @@
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B296">
         <v>400009</v>
@@ -3661,7 +3661,7 @@
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B297">
         <v>400010</v>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B298">
         <v>400011</v>
@@ -3677,7 +3677,7 @@
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B299">
         <v>400012</v>
@@ -3685,7 +3685,7 @@
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B300">
         <v>400013</v>
@@ -3693,7 +3693,7 @@
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B301">
         <v>400014</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B302">
         <v>400015</v>
@@ -3709,7 +3709,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B303">
         <v>400016</v>
@@ -3717,7 +3717,7 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B304">
         <v>400017</v>
@@ -3725,7 +3725,7 @@
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B305">
         <v>400018</v>
@@ -3733,7 +3733,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B306">
         <v>400019</v>
@@ -3741,7 +3741,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B307">
         <v>400020</v>
@@ -3749,7 +3749,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B308">
         <v>400021</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B309">
         <v>400042</v>
@@ -3765,7 +3765,7 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B310">
         <v>400043</v>
@@ -3773,7 +3773,7 @@
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B311">
         <v>400044</v>
@@ -3781,7 +3781,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B312">
         <v>400045</v>
@@ -3789,7 +3789,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B313">
         <v>400046</v>
@@ -3797,7 +3797,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B314">
         <v>400047</v>
@@ -3805,7 +3805,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B315">
         <v>400048</v>
@@ -3818,7 +3818,7 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B317">
         <v>500001</v>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B318">
         <v>500002</v>
@@ -3834,7 +3834,7 @@
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B319">
         <v>500003</v>

</xml_diff>